<commit_message>
Excel comparison of burn time estimations
</commit_message>
<xml_diff>
--- a/Burn-time calculation.xlsx
+++ b/Burn-time calculation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>R</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>ISP*G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total delta-v = </t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>burn dv</t>
+  </si>
+  <si>
+    <t>finmass</t>
+  </si>
+  <si>
+    <t>avg acce</t>
+  </si>
+  <si>
+    <t>MJ time</t>
   </si>
 </sst>
 </file>
@@ -465,15 +483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +505,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,8 +518,11 @@
       <c r="E2">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="D3" t="s">
@@ -510,8 +531,11 @@
       <c r="E3">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -525,7 +549,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -533,7 +557,7 @@
         <v>661690</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -547,16 +571,23 @@
         <f>E1*E2</f>
         <v>2109.15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>-23.599699999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>E1*E2*LN(E3/G3)</f>
+        <v>1725.9392188394504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -564,8 +595,11 @@
         <f>SQRT(B4^2+B5^2)</f>
         <v>669078.44462663715</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -573,8 +607,12 @@
         <f>B9-B1</f>
         <v>69078.444626637152</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>SQRT(B2/B15)*(1-SQRT(1-B14))</f>
+        <v>1545.0591677879884</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -583,7 +621,13 @@
         <v>757.29351057603822</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>G10/G7</f>
+        <v>0.89519906084926404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -594,8 +638,15 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <f>E3/EXP(LN(E3/G3)*H12)</f>
+        <v>0.49029501099155071</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -608,13 +659,29 @@
         <v>22.344545551343415</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15">
         <f>B13*(1+B14)</f>
         <v>669639.12567228905</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15">
+        <f>E4/((E3+H13)/2)</f>
+        <v>66.212229579138466</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <f>G10/H15</f>
+        <v>23.334951527969558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>